<commit_message>
File cleanup and correct state dropdowns
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathaniyer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-oregon\InputData\elec\MCGLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1633845B-D212-7F4E-84E3-60B256834DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="840" windowWidth="15520" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3683" yWindow="840" windowWidth="15518" windowHeight="14423"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="6" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="percentile">About!$A$68</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -415,7 +414,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -540,7 +539,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,23 +630,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -683,23 +665,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -875,25 +840,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="6" customWidth="1"/>
-    <col min="2" max="4" width="55.83203125" style="6" customWidth="1"/>
+    <col min="2" max="4" width="55.796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>124</v>
@@ -902,10 +867,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="str">
         <f>LOOKUP(B1,E2:F51,F2:F51)</f>
-        <v>VA</v>
+        <v>OR</v>
       </c>
       <c r="C2" s="6">
         <f>LOOKUP(B1,E2:G51,G2:G51)</f>
@@ -921,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="9" t="s">
         <v>119</v>
       </c>
@@ -932,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
@@ -949,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="9" t="s">
         <v>77</v>
       </c>
@@ -960,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>121</v>
       </c>
@@ -974,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>122</v>
       </c>
@@ -988,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E8" s="9" t="s">
         <v>86</v>
       </c>
@@ -999,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>123</v>
       </c>
@@ -1013,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E10" s="9" t="s">
         <v>87</v>
       </c>
@@ -1024,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E11" s="9" t="s">
         <v>88</v>
       </c>
@@ -1035,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E12" s="9" t="s">
         <v>48</v>
       </c>
@@ -1046,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E13" s="9" t="s">
         <v>75</v>
       </c>
@@ -1057,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1071,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E15" s="9" t="s">
         <v>66</v>
       </c>
@@ -1082,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E16" s="9" t="s">
         <v>76</v>
       </c>
@@ -1093,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E17" s="9" t="s">
         <v>90</v>
       </c>
@@ -1104,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E18" s="9" t="s">
         <v>91</v>
       </c>
@@ -1115,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E19" s="9" t="s">
         <v>92</v>
       </c>
@@ -1126,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E20" s="9" t="s">
         <v>93</v>
       </c>
@@ -1137,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E21" s="9" t="s">
         <v>94</v>
       </c>
@@ -1148,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E22" s="9" t="s">
         <v>95</v>
       </c>
@@ -1159,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E23" s="9" t="s">
         <v>96</v>
       </c>
@@ -1170,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E24" s="9" t="s">
         <v>97</v>
       </c>
@@ -1181,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E25" s="9" t="s">
         <v>36</v>
       </c>
@@ -1192,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E26" s="9" t="s">
         <v>98</v>
       </c>
@@ -1203,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E27" s="9" t="s">
         <v>99</v>
       </c>
@@ -1214,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="16"/>
       <c r="E28" s="9" t="s">
         <v>100</v>
@@ -1226,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -1240,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -1254,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -1268,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="16"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1283,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -1297,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="16"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -1312,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="20"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -1327,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="16"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
@@ -1342,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="20"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -1357,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="16"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -1372,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="20"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -1387,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -1401,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -1415,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E42" s="9" t="s">
         <v>110</v>
       </c>
@@ -1426,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E43" s="9" t="s">
         <v>111</v>
       </c>
@@ -1437,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="16"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
@@ -1452,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="20"/>
       <c r="E45" s="9" t="s">
         <v>71</v>
@@ -1464,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="20"/>
       <c r="E46" s="9" t="s">
         <v>112</v>
@@ -1476,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="20"/>
       <c r="E47" s="9" t="s">
         <v>55</v>
@@ -1488,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="20"/>
       <c r="E48" s="9" t="s">
         <v>25</v>
@@ -1500,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E49" s="9" t="s">
         <v>113</v>
       </c>
@@ -1511,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E50" s="9" t="s">
         <v>114</v>
       </c>
@@ -1522,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E51" s="9" t="s">
         <v>74</v>
       </c>
@@ -1533,49 +1498,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="16"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="16"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="16"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="16"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="16"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="16"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="16"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="16"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="16"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="16"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="16"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="16"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="16"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="22"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="16"/>
     </row>
   </sheetData>
@@ -1585,7 +1550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1595,19 +1560,19 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>79</v>
       </c>
@@ -1621,7 +1586,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A2" s="11"/>
       <c r="B2" s="1" t="s">
         <v>118</v>
@@ -1634,7 +1599,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
@@ -1648,7 +1613,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>118</v>
@@ -1661,7 +1626,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1675,7 +1640,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>118</v>
@@ -1688,7 +1653,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1702,7 +1667,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
         <v>118</v>
@@ -1722,7 +1687,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
@@ -1744,7 +1709,7 @@
       <c r="K9" s="8"/>
       <c r="AW9" s="3"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A10" s="11"/>
       <c r="B10" s="1" t="s">
         <v>118</v>
@@ -1763,7 +1728,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
@@ -1811,7 +1776,7 @@
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A12" s="11"/>
       <c r="B12" s="1" t="s">
         <v>118</v>
@@ -1858,7 +1823,7 @@
       <c r="AK12" s="5"/>
       <c r="AL12" s="5"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
@@ -1905,7 +1870,7 @@
       <c r="AQ13" s="6"/>
       <c r="AR13" s="6"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
         <v>118</v>
@@ -1918,7 +1883,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1897,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>118</v>
@@ -1945,7 +1910,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1959,7 +1924,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>118</v>
@@ -1972,7 +1937,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>15</v>
       </c>
@@ -1986,7 +1951,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="11"/>
       <c r="B20" s="1" t="s">
         <v>118</v>
@@ -1999,7 +1964,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
@@ -2013,7 +1978,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>118</v>
@@ -2026,7 +1991,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>80</v>
       </c>
@@ -2040,7 +2005,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>118</v>
@@ -2053,7 +2018,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>81</v>
       </c>
@@ -2068,7 +2033,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="11"/>
       <c r="B26" s="1" t="s">
         <v>118</v>
@@ -2083,7 +2048,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>115</v>
       </c>
@@ -2098,7 +2063,7 @@
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="11"/>
       <c r="B28" s="1" t="s">
         <v>118</v>
@@ -2110,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>116</v>
       </c>
@@ -2124,7 +2089,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="11"/>
       <c r="B30" s="1" t="s">
         <v>118</v>
@@ -2136,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>117</v>
       </c>
@@ -2150,7 +2115,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="11"/>
       <c r="B32" s="1" t="s">
         <v>118</v>

</xml_diff>